<commit_message>
Desarrollando distribucion de utilidades Se cargn en tiempo real los excel de los reportes
</commit_message>
<xml_diff>
--- a/app-RRHH/file/resumen_detalle_min.xlsx
+++ b/app-RRHH/file/resumen_detalle_min.xlsx
@@ -667,8 +667,8 @@
   </sheetPr>
   <dimension ref="B1:AI268"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U3" activeCellId="0" sqref="U3:U268"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X10" activeCellId="0" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.18359375" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>
@@ -688,13 +688,13 @@
     <col width="9.27" customWidth="1" style="17" min="18" max="18"/>
     <col width="4.73" customWidth="1" style="17" min="19" max="19"/>
     <col width="9.18" customWidth="1" style="17" min="20" max="20"/>
-    <col width="6.73" customWidth="1" style="17" min="21" max="21"/>
+    <col width="11.96" customWidth="1" style="17" min="21" max="21"/>
     <col width="10.85" customWidth="1" style="17" min="22" max="22"/>
     <col width="6.82" customWidth="1" style="17" min="23" max="25"/>
     <col width="9.27" customWidth="1" style="17" min="26" max="26"/>
     <col width="4.73" customWidth="1" style="17" min="27" max="27"/>
     <col width="11.7" customWidth="1" style="17" min="28" max="28"/>
-    <col width="6.73" customWidth="1" style="17" min="29" max="29"/>
+    <col width="10.29" customWidth="1" style="17" min="29" max="29"/>
     <col width="10.71" customWidth="1" style="17" min="30" max="30"/>
     <col width="6.82" customWidth="1" style="17" min="31" max="33"/>
     <col width="9.27" customWidth="1" style="17" min="34" max="34"/>
@@ -5349,7 +5349,7 @@
         </is>
       </c>
       <c r="AC51" t="n">
-        <v>666.26</v>
+        <v>0</v>
       </c>
       <c r="AD51" t="n">
         <v>5815.61</v>
@@ -5440,7 +5440,7 @@
         </is>
       </c>
       <c r="AC52" t="n">
-        <v>237.96</v>
+        <v>0</v>
       </c>
       <c r="AD52" t="n">
         <v>4976.96</v>
@@ -5531,7 +5531,7 @@
         </is>
       </c>
       <c r="AC53" t="n">
-        <v>570.86</v>
+        <v>0</v>
       </c>
       <c r="AD53" t="n">
         <v>5323.61</v>
@@ -5618,7 +5618,7 @@
         </is>
       </c>
       <c r="AC54" t="n">
-        <v>527.7</v>
+        <v>0</v>
       </c>
       <c r="AD54" t="n">
         <v>5286.4</v>
@@ -5796,7 +5796,7 @@
         </is>
       </c>
       <c r="AC56" t="n">
-        <v>324.27</v>
+        <v>0</v>
       </c>
       <c r="AD56" t="n">
         <v>5061.47</v>
@@ -5887,7 +5887,7 @@
         </is>
       </c>
       <c r="AC57" t="n">
-        <v>318.42</v>
+        <v>0</v>
       </c>
       <c r="AD57" t="n">
         <v>5439.62</v>
@@ -5978,7 +5978,7 @@
         </is>
       </c>
       <c r="AC58" t="n">
-        <v>626.34</v>
+        <v>0</v>
       </c>
       <c r="AD58" t="n">
         <v>5345.24</v>
@@ -6065,7 +6065,7 @@
         </is>
       </c>
       <c r="AC59" t="n">
-        <v>503.04</v>
+        <v>0</v>
       </c>
       <c r="AD59" t="n">
         <v>5261.74</v>
@@ -6417,7 +6417,7 @@
         </is>
       </c>
       <c r="AC63" t="n">
-        <v>505.72</v>
+        <v>0</v>
       </c>
       <c r="AD63" t="n">
         <v>5656.92</v>
@@ -6595,7 +6595,7 @@
         </is>
       </c>
       <c r="AC65" t="n">
-        <v>16.03</v>
+        <v>0</v>
       </c>
       <c r="AD65" t="n">
         <v>4767.83</v>
@@ -6686,7 +6686,7 @@
         </is>
       </c>
       <c r="AC66" t="n">
-        <v>1000.73</v>
+        <v>0</v>
       </c>
       <c r="AD66" t="n">
         <v>6120.68</v>
@@ -6777,7 +6777,7 @@
         </is>
       </c>
       <c r="AC67" t="n">
-        <v>652.89</v>
+        <v>0</v>
       </c>
       <c r="AD67" t="n">
         <v>5771.79</v>
@@ -6959,7 +6959,7 @@
         </is>
       </c>
       <c r="AC69" t="n">
-        <v>920.46</v>
+        <v>0</v>
       </c>
       <c r="AD69" t="n">
         <v>6042.86</v>
@@ -7315,7 +7315,7 @@
         </is>
       </c>
       <c r="AC73" t="n">
-        <v>293.44</v>
+        <v>0</v>
       </c>
       <c r="AD73" t="n">
         <v>5004.24</v>
@@ -7916,7 +7916,7 @@
         </is>
       </c>
       <c r="U80" t="n">
-        <v>404.2</v>
+        <v>6352.67</v>
       </c>
       <c r="V80" t="n">
         <v>12326.12</v>
@@ -7932,7 +7932,7 @@
         </is>
       </c>
       <c r="AC80" t="n">
-        <v>0</v>
+        <v>4448.88</v>
       </c>
       <c r="AD80" t="n">
         <v>9527.58</v>
@@ -8003,7 +8003,7 @@
         </is>
       </c>
       <c r="U81" t="n">
-        <v>390.07</v>
+        <v>4102.22</v>
       </c>
       <c r="V81" t="n">
         <v>10061.54</v>
@@ -8019,7 +8019,7 @@
         </is>
       </c>
       <c r="AC81" t="n">
-        <v>0</v>
+        <v>3360.09</v>
       </c>
       <c r="AD81" t="n">
         <v>8438.790000000001</v>
@@ -8090,7 +8090,7 @@
         <v>1532</v>
       </c>
       <c r="U82" t="n">
-        <v>527.26</v>
+        <v>0</v>
       </c>
       <c r="V82" t="n">
         <v>6578.68</v>
@@ -8272,7 +8272,7 @@
         </is>
       </c>
       <c r="U84" t="n">
-        <v>332.04</v>
+        <v>11538.1</v>
       </c>
       <c r="V84" t="n">
         <v>17844.43</v>
@@ -8288,7 +8288,7 @@
         </is>
       </c>
       <c r="AC84" t="n">
-        <v>0</v>
+        <v>10579.67</v>
       </c>
       <c r="AD84" t="n">
         <v>16027.73</v>
@@ -8486,7 +8486,7 @@
         </is>
       </c>
       <c r="AC86" t="n">
-        <v>0</v>
+        <v>3007.12</v>
       </c>
       <c r="AD86" t="n">
         <v>8085.82</v>
@@ -8660,7 +8660,7 @@
         </is>
       </c>
       <c r="U88" t="n">
-        <v>323.3</v>
+        <v>6212.08</v>
       </c>
       <c r="V88" t="n">
         <v>13522.26</v>
@@ -8676,7 +8676,7 @@
         </is>
       </c>
       <c r="AC88" t="n">
-        <v>0</v>
+        <v>6158.64</v>
       </c>
       <c r="AD88" t="n">
         <v>12530.1</v>
@@ -9198,7 +9198,7 @@
         </is>
       </c>
       <c r="U94" t="n">
-        <v>242.47</v>
+        <v>836.3099999999999</v>
       </c>
       <c r="V94" t="n">
         <v>6648.03</v>
@@ -9214,7 +9214,7 @@
         </is>
       </c>
       <c r="AC94" t="n">
-        <v>0</v>
+        <v>-323.19</v>
       </c>
       <c r="AD94" t="n">
         <v>946.48</v>
@@ -9289,7 +9289,7 @@
         </is>
       </c>
       <c r="U95" t="n">
-        <v>207.12</v>
+        <v>520.52</v>
       </c>
       <c r="V95" t="n">
         <v>5517.78</v>
@@ -9305,7 +9305,7 @@
         </is>
       </c>
       <c r="AC95" t="n">
-        <v>0</v>
+        <v>-257.08</v>
       </c>
       <c r="AD95" t="n">
         <v>752.89</v>
@@ -9380,7 +9380,7 @@
         </is>
       </c>
       <c r="U96" t="n">
-        <v>408.25</v>
+        <v>13719.94</v>
       </c>
       <c r="V96" t="n">
         <v>20102.48</v>
@@ -9396,7 +9396,7 @@
         </is>
       </c>
       <c r="AC96" t="n">
-        <v>0</v>
+        <v>9440.370000000001</v>
       </c>
       <c r="AD96" t="n">
         <v>14857.47</v>
@@ -9471,7 +9471,7 @@
         </is>
       </c>
       <c r="U97" t="n">
-        <v>619.02</v>
+        <v>9184.27</v>
       </c>
       <c r="V97" t="n">
         <v>15777.58</v>
@@ -9487,7 +9487,7 @@
         </is>
       </c>
       <c r="AC97" t="n">
-        <v>0</v>
+        <v>10473.24</v>
       </c>
       <c r="AD97" t="n">
         <v>15395.07</v>
@@ -9566,7 +9566,7 @@
         </is>
       </c>
       <c r="U98" t="n">
-        <v>0</v>
+        <v>-1351.52</v>
       </c>
       <c r="V98" t="n">
         <v>3958.03</v>
@@ -9582,7 +9582,7 @@
         </is>
       </c>
       <c r="AC98" t="n">
-        <v>0</v>
+        <v>-126.99</v>
       </c>
       <c r="AD98" t="n">
         <v>1402.39</v>
@@ -9681,7 +9681,7 @@
         </is>
       </c>
       <c r="AC99" t="n">
-        <v>0</v>
+        <v>18.43</v>
       </c>
       <c r="AD99" t="n">
         <v>3567.75</v>
@@ -9780,7 +9780,7 @@
         </is>
       </c>
       <c r="AC100" t="n">
-        <v>0</v>
+        <v>-448.06</v>
       </c>
       <c r="AD100" t="n">
         <v>1312.17</v>
@@ -9855,7 +9855,7 @@
         </is>
       </c>
       <c r="U101" t="n">
-        <v>0</v>
+        <v>17560.1</v>
       </c>
       <c r="V101" t="n">
         <v>23008.16</v>
@@ -9871,7 +9871,7 @@
         </is>
       </c>
       <c r="AC101" t="n">
-        <v>0</v>
+        <v>10126.22</v>
       </c>
       <c r="AD101" t="n">
         <v>15574.28</v>
@@ -9938,7 +9938,7 @@
         <v>1838.4</v>
       </c>
       <c r="U102" t="n">
-        <v>525.78</v>
+        <v>0</v>
       </c>
       <c r="V102" t="n">
         <v>7917.7</v>
@@ -10025,7 +10025,7 @@
         </is>
       </c>
       <c r="U103" t="n">
-        <v>613</v>
+        <v>3402.61</v>
       </c>
       <c r="V103" t="n">
         <v>9989.9</v>
@@ -10041,7 +10041,7 @@
         </is>
       </c>
       <c r="AC103" t="n">
-        <v>0</v>
+        <v>13510.98</v>
       </c>
       <c r="AD103" t="n">
         <v>18680.44</v>
@@ -10112,7 +10112,7 @@
         </is>
       </c>
       <c r="U104" t="n">
-        <v>352.97</v>
+        <v>4541.54</v>
       </c>
       <c r="V104" t="n">
         <v>10868.8</v>
@@ -10128,7 +10128,7 @@
         </is>
       </c>
       <c r="AC104" t="n">
-        <v>0</v>
+        <v>2268.86</v>
       </c>
       <c r="AD104" t="n">
         <v>7716.92</v>
@@ -10199,7 +10199,7 @@
         </is>
       </c>
       <c r="U105" t="n">
-        <v>390.93</v>
+        <v>1614.89</v>
       </c>
       <c r="V105" t="n">
         <v>5287.04</v>
@@ -10211,7 +10211,7 @@
         <v>1238.2</v>
       </c>
       <c r="AC105" t="n">
-        <v>0</v>
+        <v>2434.32</v>
       </c>
       <c r="AD105" t="n">
         <v>4322.57</v>
@@ -10282,7 +10282,7 @@
         <v>1981.11</v>
       </c>
       <c r="U106" t="n">
-        <v>594.83</v>
+        <v>6478.62</v>
       </c>
       <c r="V106" t="n">
         <v>10849.95</v>
@@ -10294,7 +10294,7 @@
         <v>1238.2</v>
       </c>
       <c r="AC106" t="n">
-        <v>0</v>
+        <v>644.5700000000001</v>
       </c>
       <c r="AD106" t="n">
         <v>923.16</v>
@@ -10365,7 +10365,7 @@
         <v>2606.51</v>
       </c>
       <c r="U107" t="n">
-        <v>336.78</v>
+        <v>9637.309999999999</v>
       </c>
       <c r="V107" t="n">
         <v>16960.97</v>
@@ -10381,7 +10381,7 @@
         </is>
       </c>
       <c r="AC107" t="n">
-        <v>0</v>
+        <v>5925.8</v>
       </c>
       <c r="AD107" t="n">
         <v>9726.950000000001</v>
@@ -10452,7 +10452,7 @@
         <v>1981.11</v>
       </c>
       <c r="U108" t="n">
-        <v>407.39</v>
+        <v>446.29</v>
       </c>
       <c r="V108" t="n">
         <v>5209.95</v>
@@ -10468,7 +10468,7 @@
         </is>
       </c>
       <c r="AC108" t="n">
-        <v>0</v>
+        <v>2166.48</v>
       </c>
       <c r="AD108" t="n">
         <v>6126.73</v>
@@ -10539,7 +10539,7 @@
         <v>1485.84</v>
       </c>
       <c r="U109" t="n">
-        <v>476.13</v>
+        <v>11129.93</v>
       </c>
       <c r="V109" t="n">
         <v>16218.34</v>
@@ -10555,7 +10555,7 @@
         </is>
       </c>
       <c r="AC109" t="n">
-        <v>0</v>
+        <v>7258.99</v>
       </c>
       <c r="AD109" t="n">
         <v>12707.05</v>
@@ -10626,7 +10626,7 @@
         <v>1238.2</v>
       </c>
       <c r="U110" t="n">
-        <v>285.54</v>
+        <v>3249.26</v>
       </c>
       <c r="V110" t="n">
         <v>7868.48</v>
@@ -10642,7 +10642,7 @@
         </is>
       </c>
       <c r="AC110" t="n">
-        <v>0</v>
+        <v>3911.17</v>
       </c>
       <c r="AD110" t="n">
         <v>9359.23</v>
@@ -10713,7 +10713,7 @@
         <v>1238.2</v>
       </c>
       <c r="U111" t="n">
-        <v>321.7</v>
+        <v>2104.82</v>
       </c>
       <c r="V111" t="n">
         <v>6760.2</v>
@@ -10729,7 +10729,7 @@
         </is>
       </c>
       <c r="AC111" t="n">
-        <v>0</v>
+        <v>-1407.87</v>
       </c>
       <c r="AD111" t="n">
         <v>4040.19</v>
@@ -10800,7 +10800,7 @@
         <v>1238.2</v>
       </c>
       <c r="U112" t="n">
-        <v>195.83</v>
+        <v>2266.74</v>
       </c>
       <c r="V112" t="n">
         <v>5465.19</v>
@@ -10895,7 +10895,7 @@
         </is>
       </c>
       <c r="U113" t="n">
-        <v>524.6</v>
+        <v>12248.91</v>
       </c>
       <c r="V113" t="n">
         <v>18747.8</v>
@@ -10907,7 +10907,7 @@
         <v>1485.84</v>
       </c>
       <c r="AC113" t="n">
-        <v>0</v>
+        <v>8164.86</v>
       </c>
       <c r="AD113" t="n">
         <v>12250.9</v>
@@ -10982,7 +10982,7 @@
         </is>
       </c>
       <c r="U114" t="n">
-        <v>254.1</v>
+        <v>3359.26</v>
       </c>
       <c r="V114" t="n">
         <v>8777.58</v>
@@ -10994,7 +10994,7 @@
         <v>1284.36</v>
       </c>
       <c r="AC114" t="n">
-        <v>0</v>
+        <v>595.85</v>
       </c>
       <c r="AD114" t="n">
         <v>4127.85</v>
@@ -11069,7 +11069,7 @@
         </is>
       </c>
       <c r="U115" t="n">
-        <v>0</v>
+        <v>9526.209999999999</v>
       </c>
       <c r="V115" t="n">
         <v>16141.2</v>
@@ -11081,7 +11081,7 @@
         <v>1485.84</v>
       </c>
       <c r="AC115" t="n">
-        <v>0</v>
+        <v>533.3</v>
       </c>
       <c r="AD115" t="n">
         <v>4493.55</v>
@@ -11156,7 +11156,7 @@
         </is>
       </c>
       <c r="U116" t="n">
-        <v>170.83</v>
+        <v>4014.75</v>
       </c>
       <c r="V116" t="n">
         <v>9495.129999999999</v>
@@ -11172,7 +11172,7 @@
         </is>
       </c>
       <c r="AC116" t="n">
-        <v>0</v>
+        <v>-822.65</v>
       </c>
       <c r="AD116" t="n">
         <v>4256.05</v>
@@ -11247,7 +11247,7 @@
         </is>
       </c>
       <c r="U117" t="n">
-        <v>767.4299999999999</v>
+        <v>11544.5</v>
       </c>
       <c r="V117" t="n">
         <v>18286.22</v>
@@ -11263,7 +11263,7 @@
         </is>
       </c>
       <c r="AC117" t="n">
-        <v>0</v>
+        <v>8996.700000000001</v>
       </c>
       <c r="AD117" t="n">
         <v>14444.76</v>
@@ -11338,7 +11338,7 @@
         </is>
       </c>
       <c r="U118" t="n">
-        <v>338.46</v>
+        <v>4043.5</v>
       </c>
       <c r="V118" t="n">
         <v>11368.84</v>
@@ -11354,7 +11354,7 @@
         </is>
       </c>
       <c r="AC118" t="n">
-        <v>0</v>
+        <v>751.1</v>
       </c>
       <c r="AD118" t="n">
         <v>7122.56</v>
@@ -11429,7 +11429,7 @@
         </is>
       </c>
       <c r="U119" t="n">
-        <v>270.63</v>
+        <v>2664.21</v>
       </c>
       <c r="V119" t="n">
         <v>7390.24</v>
@@ -11445,7 +11445,7 @@
         </is>
       </c>
       <c r="AC119" t="n">
-        <v>0</v>
+        <v>534.33</v>
       </c>
       <c r="AD119" t="n">
         <v>4597.29</v>
@@ -11607,7 +11607,7 @@
         </is>
       </c>
       <c r="U121" t="n">
-        <v>230</v>
+        <v>2520.04</v>
       </c>
       <c r="V121" t="n">
         <v>8319.290000000001</v>
@@ -11623,7 +11623,7 @@
         </is>
       </c>
       <c r="AC121" t="n">
-        <v>0</v>
+        <v>882.89</v>
       </c>
       <c r="AD121" t="n">
         <v>5701.88</v>
@@ -11698,7 +11698,7 @@
         </is>
       </c>
       <c r="U122" t="n">
-        <v>268.24</v>
+        <v>3997.93</v>
       </c>
       <c r="V122" t="n">
         <v>9835.42</v>
@@ -11714,7 +11714,7 @@
         </is>
       </c>
       <c r="AC122" t="n">
-        <v>0</v>
+        <v>3904.89</v>
       </c>
       <c r="AD122" t="n">
         <v>8723.879999999999</v>
@@ -12074,7 +12074,7 @@
         </is>
       </c>
       <c r="AC126" t="n">
-        <v>564.6900000000001</v>
+        <v>0</v>
       </c>
       <c r="AD126" t="n">
         <v>5305.99</v>
@@ -14087,7 +14087,7 @@
         </is>
       </c>
       <c r="U149" t="n">
-        <v>252.61</v>
+        <v>2826.47</v>
       </c>
       <c r="V149" t="n">
         <v>7690.84</v>
@@ -15329,7 +15329,7 @@
         </is>
       </c>
       <c r="AC163" t="n">
-        <v>1168.84</v>
+        <v>0</v>
       </c>
       <c r="AD163" t="n">
         <v>5912.64</v>
@@ -19423,7 +19423,7 @@
         <v>2971.67</v>
       </c>
       <c r="U209" t="n">
-        <v>244.82</v>
+        <v>922.65</v>
       </c>
       <c r="V209" t="n">
         <v>7358.45</v>
@@ -19439,7 +19439,7 @@
         </is>
       </c>
       <c r="AC209" t="n">
-        <v>0</v>
+        <v>104.12</v>
       </c>
       <c r="AD209" t="n">
         <v>2704.33</v>
@@ -20483,7 +20483,7 @@
         <v>2971.67</v>
       </c>
       <c r="U221" t="n">
-        <v>260.41</v>
+        <v>503.39</v>
       </c>
       <c r="V221" t="n">
         <v>6707.14</v>
@@ -20495,7 +20495,7 @@
         <v>1485.84</v>
       </c>
       <c r="AC221" t="n">
-        <v>0</v>
+        <v>659.75</v>
       </c>
       <c r="AD221" t="n">
         <v>1278.85</v>
@@ -21211,7 +21211,7 @@
         </is>
       </c>
       <c r="AC229" t="n">
-        <v>1288.38</v>
+        <v>0</v>
       </c>
       <c r="AD229" t="n">
         <v>6392.28</v>
@@ -21286,7 +21286,7 @@
         </is>
       </c>
       <c r="U230" t="n">
-        <v>226.19</v>
+        <v>-1469.05</v>
       </c>
       <c r="V230" t="n">
         <v>4528.39</v>
@@ -21302,7 +21302,7 @@
         </is>
       </c>
       <c r="AC230" t="n">
-        <v>0</v>
+        <v>735.83</v>
       </c>
       <c r="AD230" t="n">
         <v>5929.95</v>
@@ -21749,7 +21749,7 @@
         </is>
       </c>
       <c r="AC235" t="n">
-        <v>893.7</v>
+        <v>0</v>
       </c>
       <c r="AD235" t="n">
         <v>6006.65</v>
@@ -22825,7 +22825,7 @@
         </is>
       </c>
       <c r="U247" t="n">
-        <v>256.21</v>
+        <v>2784.8</v>
       </c>
       <c r="V247" t="n">
         <v>6291.27</v>
@@ -22841,7 +22841,7 @@
         </is>
       </c>
       <c r="AC247" t="n">
-        <v>0</v>
+        <v>-1342.69</v>
       </c>
       <c r="AD247" t="n">
         <v>4105.37</v>
@@ -23806,7 +23806,7 @@
         <v>1238.2</v>
       </c>
       <c r="U258" t="n">
-        <v>363.66</v>
+        <v>1943.63</v>
       </c>
       <c r="V258" t="n">
         <v>6888.61</v>
@@ -23822,7 +23822,7 @@
         </is>
       </c>
       <c r="AC258" t="n">
-        <v>0</v>
+        <v>1889.46</v>
       </c>
       <c r="AD258" t="n">
         <v>7461.34</v>
@@ -23913,7 +23913,7 @@
         </is>
       </c>
       <c r="AC259" t="n">
-        <v>64.22</v>
+        <v>0</v>
       </c>
       <c r="AD259" t="n">
         <v>5166.32</v>
@@ -24746,7 +24746,7 @@
   <dimension ref="C4:C5"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H10" activeCellId="1" sqref="U3:U268 H10"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.6328125" defaultRowHeight="14.25" zeroHeight="0" outlineLevelRow="0"/>

</xml_diff>